<commit_message>
Data Collection, Cleaning, and Processing Complete
</commit_message>
<xml_diff>
--- a/Project Progress/References.xlsx
+++ b/Project Progress/References.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8fd1bd11cd8af38/Documents/University Documents/MSc Data Science/09-Data-Science-Project/Project Diary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8fd1bd11cd8af38/Documents/University Documents/MSc Data Science/09-Data-Science-Project/Project/project progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_F25DC773A252ABDACC104848419859645ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79F000D5-9B15-4206-AF5C-AA98E16F179D}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC104848419859645ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4EC99A3-CE69-4797-8212-9E8BF93A63A5}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="3300" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -133,6 +133,87 @@
   </si>
   <si>
     <t>Used to create database schema</t>
+  </si>
+  <si>
+    <t>Nas Introduced by Coercion</t>
+  </si>
+  <si>
+    <t>https://statisticsglobe.com/warning-message-nas-introduced-by-coercion-in-r</t>
+  </si>
+  <si>
+    <t>Used to solve an issue when coercing data to the correct data type where lots of warnings would be thrown.</t>
+  </si>
+  <si>
+    <t>Remove periods/dots in entire data frame</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/55026965/remove-periods-dots-in-entire-data-frame</t>
+  </si>
+  <si>
+    <t>Used to develop method to remove thousand seperators from values in dataframes</t>
+  </si>
+  <si>
+    <t>https://dplyr.tidyverse.org/reference/relocate.html</t>
+  </si>
+  <si>
+    <t>Change column order</t>
+  </si>
+  <si>
+    <t>Used to have a more elegant method of reordering columns than using a select</t>
+  </si>
+  <si>
+    <t>Remove all special characters from a string in R</t>
+  </si>
+  <si>
+    <t>https://intellipaat.com/community/15034/remove-all-special-characters-from-a-string-in-r</t>
+  </si>
+  <si>
+    <t>Used to clean first names from person dataframe</t>
+  </si>
+  <si>
+    <t>genderizeR</t>
+  </si>
+  <si>
+    <t>https://github.com/kalimu/genderizeR</t>
+  </si>
+  <si>
+    <t>Package used to access the genderize API easily and process names - detailed citation available on the page</t>
+  </si>
+  <si>
+    <t>R for Data Science - Data Import - Parsering a vector</t>
+  </si>
+  <si>
+    <t>https://r4ds.had.co.nz/data-import.html#parsing-a-vector</t>
+  </si>
+  <si>
+    <t>Used to solve an encoding issues with names</t>
+  </si>
+  <si>
+    <t>How to plot multiple data series in GGPLOT</t>
+  </si>
+  <si>
+    <t>https://www.sixhat.net/how-to-plot-multpile-data-series-with-ggplot.html</t>
+  </si>
+  <si>
+    <t>Used to plot two data series to the same graph and have a legend show</t>
+  </si>
+  <si>
+    <t>Relational Data</t>
+  </si>
+  <si>
+    <t>https://r4ds.had.co.nz/relational-data.html</t>
+  </si>
+  <si>
+    <t>Used to plan out dataset schema and idenify appropriate primary and foreign keys</t>
+  </si>
+  <si>
+    <t>https://www.datanovia.com/en/blog/ggplot-legend-title-position-and-labels/</t>
+  </si>
+  <si>
+    <t>GGPlot Legend Title, Position and Labels</t>
+  </si>
+  <si>
+    <t>Used to customise plot legends</t>
   </si>
 </sst>
 </file>
@@ -485,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,6 +711,105 @@
         <v>35</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{C3894F9D-3F3D-45FC-95E3-E28747899B44}"/>
@@ -637,8 +817,11 @@
     <hyperlink ref="B3" r:id="rId3" xr:uid="{DF6F1F4F-4DF9-4131-89C7-E142575DCCAC}"/>
     <hyperlink ref="A10" r:id="rId4" display="https://stackoverflow.com/questions/14577412/how-to-convert-variable-object-name-into-string" xr:uid="{B0F6E2E9-F3ED-44AA-B8B7-51C6CCC991CD}"/>
     <hyperlink ref="B12" r:id="rId5" xr:uid="{2A462BC9-08B8-48D3-98D3-BD1380F2ECF7}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{6614E46D-B9F3-4998-B1ED-9F55A71C0D0A}"/>
+    <hyperlink ref="B15" r:id="rId7" xr:uid="{85C743E3-0EE5-4635-B409-34B38A02D5B3}"/>
+    <hyperlink ref="B21" r:id="rId8" xr:uid="{F14AD043-5A3B-4E5F-86A7-9EAE1E0CD931}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved minor data processing issues and completed data analysis plots
This commit:
- Resolves some minor data type issues with the Subject and Topic datatables, where column types were incorrect
- Adds the finalized dataset schema
- Add functionality to wrangle data into layout of database scheme
- Adds saving datasets (main and panel) as RDS object as well as CSV files.
- Adds code for the preliminary data analysis including code to wrangle the tables and code to build the plots.
- Adds weekly project update document
</commit_message>
<xml_diff>
--- a/Project Progress/References.xlsx
+++ b/Project Progress/References.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8fd1bd11cd8af38/Documents/University Documents/MSc Data Science/09-Data-Science-Project/Project/project progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC104848419859645ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4EC99A3-CE69-4797-8212-9E8BF93A63A5}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="11_F25DC773A252ABDACC104848419859645ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A72A1227-8722-4C1A-A33D-44A2E614428D}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3300" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -214,6 +214,84 @@
   </si>
   <si>
     <t>Used to customise plot legends</t>
+  </si>
+  <si>
+    <t>How to rank within groups in R</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/31859175/how-to-rank-within-groups-in-r/43666202#43666202</t>
+  </si>
+  <si>
+    <t>Used to add a rank column that had the rank of cases within groups</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/11433432/how-to-import-multiple-csv-files-at-once</t>
+  </si>
+  <si>
+    <t>How to import multiple .csv files at once</t>
+  </si>
+  <si>
+    <t>Used to load a folder of CSV files into a named list of dataframes.</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/a/51386116</t>
+  </si>
+  <si>
+    <t>Change density plot to count and scaled axis</t>
+  </si>
+  <si>
+    <t>Used to change a denisty plot to a smoothed count plot</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/40219639/how-to-deal-with-zero-in-log-plot</t>
+  </si>
+  <si>
+    <t>How to deal with zero in log plot</t>
+  </si>
+  <si>
+    <t>Used to handle log transformations on a plot when the dataset includes zeros that need plotting</t>
+  </si>
+  <si>
+    <t>GDPR Compliance for Web Scraping</t>
+  </si>
+  <si>
+    <t>https://www.zyte.com/blog/web-scraping-gdpr-compliance-guide/</t>
+  </si>
+  <si>
+    <t>Used to review and establish GDPR compliance of project and web scraping</t>
+  </si>
+  <si>
+    <t>GDPR and Research – An Overview for Researchers</t>
+  </si>
+  <si>
+    <t>https://www.ukri.org/wp-content/uploads/2020/10/UKRI-020920-GDPR-FAQs.pdf</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/22945651/remove-space-between-plotted-data-and-the-axes</t>
+  </si>
+  <si>
+    <t>Remove space between plotted data and the axes</t>
+  </si>
+  <si>
+    <t>Used to removed gaps between axis and plotted data - cleaning up axis</t>
+  </si>
+  <si>
+    <t>Editing legend (text) labels in ggplot</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/23635662/editing-legend-text-labels-in-ggplot</t>
+  </si>
+  <si>
+    <t>Used to edit legend labels for plots</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/51385455/geom-density-y-axis-goes-above-1?noredirect=1&amp;lq=1</t>
+  </si>
+  <si>
+    <t>geom_density y-axis goes above 1</t>
+  </si>
+  <si>
+    <t>Used to check density plot and then customise to actually show count curves rather than density</t>
   </si>
 </sst>
 </file>
@@ -566,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,6 +888,105 @@
         <v>62</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{C3894F9D-3F3D-45FC-95E3-E28747899B44}"/>
@@ -820,8 +997,14 @@
     <hyperlink ref="B13" r:id="rId6" xr:uid="{6614E46D-B9F3-4998-B1ED-9F55A71C0D0A}"/>
     <hyperlink ref="B15" r:id="rId7" xr:uid="{85C743E3-0EE5-4635-B409-34B38A02D5B3}"/>
     <hyperlink ref="B21" r:id="rId8" xr:uid="{F14AD043-5A3B-4E5F-86A7-9EAE1E0CD931}"/>
+    <hyperlink ref="B23" r:id="rId9" xr:uid="{FC98FDA4-765C-40D9-82C6-04DB26803C82}"/>
+    <hyperlink ref="B24" r:id="rId10" xr:uid="{282DCEC8-E7F5-4F25-9921-8CDE7A414805}"/>
+    <hyperlink ref="B28" r:id="rId11" xr:uid="{C228CD60-225F-49A9-A4AB-E04CFD4BE8AF}"/>
+    <hyperlink ref="A28" r:id="rId12" display="https://stackoverflow.com/questions/22945651/remove-space-between-plotted-data-and-the-axes" xr:uid="{5579723A-925C-4211-A99A-921DC75FA860}"/>
+    <hyperlink ref="A29" r:id="rId13" display="https://stackoverflow.com/questions/23635662/editing-legend-text-labels-in-ggplot" xr:uid="{EA8A1FAA-31B9-4E1C-A976-E525000FF1C3}"/>
+    <hyperlink ref="A30" r:id="rId14" display="https://stackoverflow.com/questions/51385455/geom-density-y-axis-goes-above-1" xr:uid="{95714F14-5FB0-4012-A1E1-CE6A27C771BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>